<commit_message>
Lit review sent to Kevin Sim and Simon Powers, now we wait and see when the review meeting is gonna be!
</commit_message>
<xml_diff>
--- a/Dissertation-Template/Gantt-Charts.xlsx
+++ b/Dissertation-Template/Gantt-Charts.xlsx
@@ -473,12 +473,12 @@
         <c:gapWidth val="95"/>
         <c:gapDepth val="95"/>
         <c:shape val="box"/>
-        <c:axId val="443853520"/>
-        <c:axId val="443855296"/>
+        <c:axId val="444485664"/>
+        <c:axId val="444487712"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="443853520"/>
+        <c:axId val="444485664"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -521,7 +521,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="443855296"/>
+        <c:crossAx val="444487712"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -529,7 +529,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="443855296"/>
+        <c:axId val="444487712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="42982.0"/>
@@ -581,7 +581,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="443853520"/>
+        <c:crossAx val="444485664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -971,7 +971,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>37.0</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.0</c:v>
@@ -1000,12 +1000,12 @@
         <c:gapWidth val="95"/>
         <c:gapDepth val="95"/>
         <c:shape val="box"/>
-        <c:axId val="328510912"/>
-        <c:axId val="328512688"/>
+        <c:axId val="327944704"/>
+        <c:axId val="327947024"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="328510912"/>
+        <c:axId val="327944704"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1042,7 +1042,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="328512688"/>
+        <c:crossAx val="327947024"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1050,7 +1050,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="328512688"/>
+        <c:axId val="327947024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="42982.0"/>
@@ -1102,7 +1102,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="328510912"/>
+        <c:crossAx val="327944704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1492,7 +1492,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>37.0</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.0</c:v>
@@ -1521,12 +1521,12 @@
         <c:gapWidth val="95"/>
         <c:gapDepth val="95"/>
         <c:shape val="box"/>
-        <c:axId val="301543776"/>
-        <c:axId val="301546096"/>
+        <c:axId val="327227824"/>
+        <c:axId val="327340112"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="301543776"/>
+        <c:axId val="327227824"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1563,7 +1563,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="301546096"/>
+        <c:crossAx val="327340112"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1571,7 +1571,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="301546096"/>
+        <c:axId val="327340112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="42982.0"/>
@@ -1623,7 +1623,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="301543776"/>
+        <c:crossAx val="327227824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2013,7 +2013,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>37.0</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.0</c:v>
@@ -2042,12 +2042,12 @@
         <c:gapWidth val="95"/>
         <c:gapDepth val="95"/>
         <c:shape val="box"/>
-        <c:axId val="301483536"/>
-        <c:axId val="330218864"/>
+        <c:axId val="299928768"/>
+        <c:axId val="299930544"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="301483536"/>
+        <c:axId val="299928768"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2084,7 +2084,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="330218864"/>
+        <c:crossAx val="299930544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2092,7 +2092,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="330218864"/>
+        <c:axId val="299930544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="42982.0"/>
@@ -2144,7 +2144,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="301483536"/>
+        <c:crossAx val="299928768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4631,7 +4631,7 @@
   <dimension ref="B2:K69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4700,19 +4700,19 @@
         <v>43044</v>
       </c>
       <c r="F4" s="7">
-        <v>43081</v>
+        <v>43052</v>
       </c>
       <c r="G4" s="8">
         <f>(F4-D4)-C4</f>
-        <v>37</v>
+        <v>8</v>
       </c>
       <c r="H4" s="8">
         <f>(F4-D4)-C4</f>
-        <v>37</v>
+        <v>8</v>
       </c>
       <c r="I4" s="8">
         <f>(F4-D4)-C4</f>
-        <v>37</v>
+        <v>8</v>
       </c>
       <c r="K4" s="1">
         <v>42982</v>

</xml_diff>

<commit_message>
Taking Jyoti's Formatting Advice
At the end of her lecture on Monday, she decided to give us a few tips about writing our dissertation. One of those was to ensure that anything before the introduction was page-numbered in Roman numerals, and the introduction section starts on the official page 1.

I've emailed her to see what she recommends for post-conclusion pages.
</commit_message>
<xml_diff>
--- a/Dissertation-Template/Gantt-Charts.xlsx
+++ b/Dissertation-Template/Gantt-Charts.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10116"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -14,23 +14,23 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
   <si>
     <t>Task</t>
   </si>
@@ -91,11 +91,23 @@
   <si>
     <t>Gantt4</t>
   </si>
+  <si>
+    <t>Add a target start date vs actual start date thing</t>
+  </si>
+  <si>
+    <t>Game Foundation I targeted Christmas and got it</t>
+  </si>
+  <si>
+    <t>And finished it on christmas day / small hours of boxing day</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Properly consider deadlines though </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -125,6 +137,7 @@
       <sz val="24"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -191,7 +204,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -230,7 +243,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -359,24 +371,24 @@
                 <c:formatCode>m/d/yy</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>42982.0</c:v>
+                  <c:v>42982</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>42982.0</c:v>
+                  <c:v>42982</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43073.0</c:v>
+                  <c:v>43073</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43101.0</c:v>
+                  <c:v>43101</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43157.0</c:v>
+                  <c:v>43157</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-0ECC-49DC-BA8D-7FB69A7CB752}"/>
             </c:ext>
@@ -439,24 +451,24 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>62.0</c:v>
+                  <c:v>62</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>91.0</c:v>
+                  <c:v>91</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>28.0</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>56.0</c:v>
+                  <c:v>56</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>28.0</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-0ECC-49DC-BA8D-7FB69A7CB752}"/>
             </c:ext>
@@ -532,7 +544,7 @@
         <c:axId val="444487712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="42982.0"/>
+          <c:min val="42982"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="t"/>
@@ -550,7 +562,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -670,7 +682,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -709,7 +721,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -838,24 +849,24 @@
                 <c:formatCode>m/d/yy</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>42982.0</c:v>
+                  <c:v>42982</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>42982.0</c:v>
+                  <c:v>42982</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43073.0</c:v>
+                  <c:v>43073</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43101.0</c:v>
+                  <c:v>43101</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43157.0</c:v>
+                  <c:v>43157</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-0ECC-49DC-BA8D-7FB69A7CB752}"/>
             </c:ext>
@@ -916,24 +927,24 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>62.0</c:v>
+                  <c:v>62</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>91.0</c:v>
+                  <c:v>91</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>28.0</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>56.0</c:v>
+                  <c:v>56</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>28.0</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-0ECC-49DC-BA8D-7FB69A7CB752}"/>
             </c:ext>
@@ -971,23 +982,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A59F-4347-BE7C-3643EA6219B5}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1053,7 +1069,7 @@
         <c:axId val="327947024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="42982.0"/>
+          <c:min val="42982"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="t"/>
@@ -1071,7 +1087,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1191,7 +1207,7 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1230,7 +1246,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1359,24 +1374,24 @@
                 <c:formatCode>m/d/yy</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>42982.0</c:v>
+                  <c:v>42982</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>42982.0</c:v>
+                  <c:v>42982</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43073.0</c:v>
+                  <c:v>43073</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43101.0</c:v>
+                  <c:v>43101</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43157.0</c:v>
+                  <c:v>43157</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-0ECC-49DC-BA8D-7FB69A7CB752}"/>
             </c:ext>
@@ -1437,24 +1452,24 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>62.0</c:v>
+                  <c:v>62</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>91.0</c:v>
+                  <c:v>91</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>28.0</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>56.0</c:v>
+                  <c:v>56</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>28.0</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-0ECC-49DC-BA8D-7FB69A7CB752}"/>
             </c:ext>
@@ -1492,23 +1507,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-ED80-AB4D-ACF4-E520B1644D96}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1574,7 +1594,7 @@
         <c:axId val="327340112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="42982.0"/>
+          <c:min val="42982"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="t"/>
@@ -1592,7 +1612,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1712,7 +1732,7 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1751,7 +1771,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1880,24 +1899,24 @@
                 <c:formatCode>m/d/yy</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>42982.0</c:v>
+                  <c:v>42982</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>42982.0</c:v>
+                  <c:v>42982</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43073.0</c:v>
+                  <c:v>43073</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43101.0</c:v>
+                  <c:v>43101</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43157.0</c:v>
+                  <c:v>43157</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-0ECC-49DC-BA8D-7FB69A7CB752}"/>
             </c:ext>
@@ -1958,24 +1977,24 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>62.0</c:v>
+                  <c:v>62</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>91.0</c:v>
+                  <c:v>91</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>28.0</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>56.0</c:v>
+                  <c:v>56</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>28.0</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-0ECC-49DC-BA8D-7FB69A7CB752}"/>
             </c:ext>
@@ -2013,23 +2032,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7FF7-BD47-B34E-31606CE789A8}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -2095,7 +2119,7 @@
         <c:axId val="299930544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="42982.0"/>
+          <c:min val="42982"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="t"/>
@@ -2113,7 +2137,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -4249,7 +4273,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -4281,7 +4311,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -4313,7 +4349,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvPr id="7" name="Chart 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -4345,7 +4387,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="8" name="Chart 7"/>
+        <xdr:cNvPr id="8" name="Chart 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -4631,7 +4679,7 @@
   <dimension ref="B2:K69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4843,7 +4891,27 @@
         <v>12</v>
       </c>
     </row>
-    <row r="29" spans="2:4" s="3" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="H13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="H14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="H15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="H17" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" s="3" customFormat="1" ht="31" x14ac:dyDescent="0.35">
       <c r="B29" s="3" t="s">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
Pushing the dissertation for no real reason
</commit_message>
<xml_diff>
--- a/Dissertation-Template/Gantt-Charts.xlsx
+++ b/Dissertation-Template/Gantt-Charts.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10116"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10319"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/x4iiiis/Documents/GitHub/HonoursProject/Dissertation-Template/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0AE7DB3-4F09-E445-9955-B74328A12CE6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="14620"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="14620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="179017" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -107,7 +108,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -377,13 +378,13 @@
                   <c:v>42982</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43073</c:v>
+                  <c:v>43095</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43101</c:v>
+                  <c:v>43184</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43157</c:v>
+                  <c:v>43187</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -454,16 +455,16 @@
                   <c:v>62</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>91</c:v>
+                  <c:v>112</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>28</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>56</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>28</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -855,13 +856,13 @@
                   <c:v>42982</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43073</c:v>
+                  <c:v>43095</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43101</c:v>
+                  <c:v>43184</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43157</c:v>
+                  <c:v>43187</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -930,16 +931,16 @@
                   <c:v>62</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>91</c:v>
+                  <c:v>112</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>28</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>56</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>28</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1380,13 +1381,13 @@
                   <c:v>42982</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43073</c:v>
+                  <c:v>43095</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43101</c:v>
+                  <c:v>43184</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43157</c:v>
+                  <c:v>43187</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1455,16 +1456,16 @@
                   <c:v>62</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>91</c:v>
+                  <c:v>112</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>28</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>56</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>28</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1513,7 +1514,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>51</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -1905,13 +1906,13 @@
                   <c:v>42982</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43073</c:v>
+                  <c:v>43095</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43101</c:v>
+                  <c:v>43184</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43157</c:v>
+                  <c:v>43187</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1980,16 +1981,16 @@
                   <c:v>62</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>91</c:v>
+                  <c:v>112</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>28</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>56</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>28</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2038,7 +2039,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>51</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -4675,11 +4676,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:K69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4772,16 +4773,16 @@
       </c>
       <c r="C5" s="6">
         <f t="shared" ref="C5:C8" si="0">E5-D5</f>
-        <v>91</v>
+        <v>112</v>
       </c>
       <c r="D5" s="7">
         <v>42982</v>
       </c>
       <c r="E5" s="7">
-        <v>43073</v>
+        <v>43094</v>
       </c>
       <c r="F5" s="7">
-        <v>43073</v>
+        <v>43094</v>
       </c>
       <c r="G5" s="8">
         <v>0</v>
@@ -4800,29 +4801,29 @@
         <v>3</v>
       </c>
       <c r="C6" s="6">
-        <f t="shared" si="0"/>
-        <v>28</v>
+        <f>E6-D6</f>
+        <v>37</v>
       </c>
       <c r="D6" s="7">
-        <f t="shared" ref="D6:D8" si="3">E5</f>
-        <v>43073</v>
+        <f>E5+1</f>
+        <v>43095</v>
       </c>
       <c r="E6" s="7">
-        <v>43101</v>
+        <v>43132</v>
       </c>
       <c r="F6" s="7">
-        <v>43101</v>
+        <v>43183</v>
       </c>
       <c r="G6" s="8">
         <v>0</v>
       </c>
       <c r="H6" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>51</v>
       </c>
       <c r="I6" s="8">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.2">
@@ -4830,18 +4831,18 @@
         <v>4</v>
       </c>
       <c r="C7" s="6">
-        <f t="shared" si="0"/>
-        <v>56</v>
+        <f>E7-D7</f>
+        <v>7</v>
       </c>
       <c r="D7" s="7">
-        <f t="shared" si="3"/>
-        <v>43101</v>
+        <f>F6+1</f>
+        <v>43184</v>
       </c>
       <c r="E7" s="7">
-        <v>43157</v>
+        <v>43191</v>
       </c>
       <c r="F7" s="7">
-        <v>43157</v>
+        <v>43191</v>
       </c>
       <c r="G7" s="8">
         <v>0</v>
@@ -4860,17 +4861,16 @@
       </c>
       <c r="C8" s="6">
         <f t="shared" si="0"/>
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="D8" s="7">
-        <f t="shared" si="3"/>
-        <v>43157</v>
+        <v>43187</v>
       </c>
       <c r="E8" s="7">
-        <v>43185</v>
+        <v>43197</v>
       </c>
       <c r="F8" s="7">
-        <v>43185</v>
+        <v>43197</v>
       </c>
       <c r="G8" s="8">
         <v>0</v>

</xml_diff>